<commit_message>
Data convert update & bag logic
</commit_message>
<xml_diff>
--- a/Data/StoreItemDefine.xlsx
+++ b/Data/StoreItemDefine.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t>ID</t>
   </si>
@@ -25,6 +25,9 @@
     <t>type</t>
   </si>
   <si>
+    <t>invokeType</t>
+  </si>
+  <si>
     <t>iconResource</t>
   </si>
   <si>
@@ -32,6 +35,12 @@
   </si>
   <si>
     <t>price</t>
+  </si>
+  <si>
+    <t>effect.effectType</t>
+  </si>
+  <si>
+    <t>effect.value</t>
   </si>
   <si>
     <t>wooden_sword_icon</t>
@@ -50,9 +59,6 @@
   </si>
   <si>
     <t>magic_sword</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -1203,19 +1209,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="184" zoomScaleNormal="184" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="6" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="6"/>
   <cols>
-    <col min="3" max="4" width="17.9326923076923" customWidth="1"/>
-    <col min="5" max="5" width="13.3173076923077" customWidth="1"/>
+    <col min="3" max="5" width="17.9326923076923" customWidth="1"/>
+    <col min="6" max="6" width="13.3173076923077" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1234,8 +1240,17 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:9">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1245,17 +1260,26 @@
       <c r="C2" s="1">
         <v>0</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
+      <c r="D2" s="1">
+        <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="1">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="1">
         <v>100</v>
       </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:9">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1265,17 +1289,26 @@
       <c r="C3" s="1">
         <v>1</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
+      <c r="D3" s="1">
+        <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="1">
+        <v>11</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="1">
         <v>200</v>
       </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
     </row>
-    <row r="4" ht="17" customHeight="1" spans="1:6">
+    <row r="4" ht="17" customHeight="1" spans="1:9">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1285,17 +1318,26 @@
       <c r="C4" s="2">
         <v>2</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>10</v>
+      <c r="D4" s="1">
+        <v>2</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="1">
+        <v>13</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="1">
         <v>400</v>
       </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <v>3</v>
+      </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:9">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1305,17 +1347,26 @@
       <c r="C5" s="1">
         <v>0</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>6</v>
+      <c r="D5" s="1">
+        <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="1">
+        <v>9</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="1">
         <v>150</v>
       </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>4</v>
+      </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:9">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1325,20 +1376,26 @@
       <c r="C6" s="1">
         <v>1</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>8</v>
+      <c r="D6" s="1">
+        <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="1">
+        <v>11</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="1">
         <v>250</v>
       </c>
-      <c r="H6" t="s">
-        <v>12</v>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>5</v>
       </c>
     </row>
-    <row r="7" ht="17" spans="1:6">
+    <row r="7" ht="17" spans="1:9">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1348,14 +1405,23 @@
       <c r="C7" s="2">
         <v>2</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>10</v>
+      <c r="D7" s="1">
+        <v>2</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="1">
+        <v>13</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="1">
         <v>450</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="I7">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
configuration & bug fix
</commit_message>
<xml_diff>
--- a/Data/StoreItemDefine.xlsx
+++ b/Data/StoreItemDefine.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="92">
   <si>
     <t>ID</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>iconResource2</t>
+  </si>
+  <si>
+    <t>targetRange</t>
   </si>
   <si>
     <t>takeEnergy</t>
@@ -1437,10 +1440,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:V30"/>
+  <dimension ref="A1:W30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="184" zoomScaleNormal="184" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="T12" sqref="T12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -1452,11 +1455,24 @@
     <col min="5" max="5" width="8.96153846153846" customWidth="1"/>
     <col min="6" max="6" width="13.3173076923077" customWidth="1"/>
     <col min="8" max="8" width="16.1923076923077" customWidth="1"/>
-    <col min="9" max="9" width="18.5384615384615" customWidth="1"/>
-    <col min="10" max="11" width="12.8846153846154" customWidth="1"/>
+    <col min="9" max="9" width="20.8269230769231" customWidth="1"/>
+    <col min="10" max="10" width="11.2115384615385" customWidth="1"/>
+    <col min="11" max="11" width="10.4807692307692" customWidth="1"/>
+    <col min="12" max="12" width="15.8942307692308" customWidth="1"/>
+    <col min="13" max="13" width="18.3653846153846" customWidth="1"/>
+    <col min="14" max="14" width="18.4903846153846" customWidth="1"/>
+    <col min="15" max="15" width="11.5769230769231" customWidth="1"/>
+    <col min="16" max="16" width="16.0192307692308" customWidth="1"/>
+    <col min="17" max="17" width="18.4807692307692" customWidth="1"/>
+    <col min="18" max="18" width="18.6057692307692" customWidth="1"/>
+    <col min="19" max="19" width="11.7019230769231" customWidth="1"/>
+    <col min="20" max="20" width="16.1442307692308" customWidth="1"/>
+    <col min="21" max="21" width="18.7307692307692" customWidth="1"/>
+    <col min="22" max="22" width="18.8653846153846" customWidth="1"/>
+    <col min="23" max="23" width="11.7019230769231" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:23">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1523,8 +1539,11 @@
       <c r="V1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:14">
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1538,31 +1557,37 @@
         <v>2</v>
       </c>
       <c r="E2" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G2" s="1">
         <v>100</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>9</v>
+      </c>
+      <c r="O2">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1576,31 +1601,37 @@
         <v>2</v>
       </c>
       <c r="E3" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G3" s="1">
         <v>200</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K3">
         <v>1</v>
       </c>
-      <c r="N3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" ht="17" customHeight="1" spans="1:14">
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>9</v>
+      </c>
+      <c r="O3">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="4" ht="17" customHeight="1" spans="1:15">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1614,31 +1645,37 @@
         <v>3</v>
       </c>
       <c r="E4" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G4" s="1">
         <v>400</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K4">
-        <v>2</v>
-      </c>
-      <c r="N4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>9</v>
+      </c>
+      <c r="O4">
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1652,25 +1689,37 @@
         <v>1</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G5">
         <v>400</v>
       </c>
       <c r="H5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="J5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+        <v>-1</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>7</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1684,25 +1733,28 @@
         <v>4</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G6">
         <v>400</v>
       </c>
       <c r="H6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+        <v>-1</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1716,25 +1768,28 @@
         <v>4</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G7">
         <v>200</v>
       </c>
       <c r="H7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+        <v>-1</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1748,25 +1803,28 @@
         <v>4</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G8">
         <v>100</v>
       </c>
       <c r="H8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
+        <v>-1</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1780,25 +1838,37 @@
         <v>3</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G9">
         <v>200</v>
       </c>
       <c r="H9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
+        <v>2</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>9</v>
+      </c>
+      <c r="O9">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1812,25 +1882,37 @@
         <v>2</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G10">
         <v>100</v>
       </c>
       <c r="H10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>9</v>
+      </c>
+      <c r="O10">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1844,25 +1926,46 @@
         <v>4</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F11" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G11">
         <v>400</v>
       </c>
       <c r="H11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
+        <v>5</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>9</v>
+      </c>
+      <c r="O11">
+        <v>-10</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>9</v>
+      </c>
+      <c r="S11">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1876,25 +1979,46 @@
         <v>1</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F12" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G12">
         <v>200</v>
       </c>
       <c r="H12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
+        <v>4</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>9</v>
+      </c>
+      <c r="O12">
+        <v>-6</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>9</v>
+      </c>
+      <c r="S12">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1908,25 +2032,37 @@
         <v>0</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F13" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G13">
         <v>100</v>
       </c>
       <c r="H13" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I13" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="J13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
+        <v>4</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>9</v>
+      </c>
+      <c r="O13">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1940,25 +2076,28 @@
         <v>1</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F14" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G14">
         <v>200</v>
       </c>
       <c r="H14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
+        <v>6</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1972,25 +2111,28 @@
         <v>1</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F15" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G15">
         <v>200</v>
       </c>
       <c r="H15" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="I15" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
+        <v>6</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -2004,25 +2146,28 @@
         <v>1</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F16" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G16">
         <v>100</v>
       </c>
       <c r="H16" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I16" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="J16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
+        <v>6</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -2036,25 +2181,28 @@
         <v>1</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F17" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G17">
         <v>100</v>
       </c>
       <c r="H17" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I17" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
+        <v>6</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -2068,25 +2216,37 @@
         <v>1</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F18" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G18">
         <v>100</v>
       </c>
       <c r="H18" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="I18" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
+        <v>6</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>9</v>
+      </c>
+      <c r="O18">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -2103,19 +2263,22 @@
         <v>2</v>
       </c>
       <c r="F19" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G19">
         <v>200</v>
       </c>
       <c r="H19" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
+        <v>-1</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -2132,19 +2295,22 @@
         <v>2</v>
       </c>
       <c r="F20" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G20">
         <v>400</v>
       </c>
       <c r="H20" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="J20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10">
+        <v>-1</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -2161,19 +2327,22 @@
         <v>2</v>
       </c>
       <c r="F21" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G21">
         <v>200</v>
       </c>
       <c r="H21" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10">
+        <v>-1</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -2190,19 +2359,22 @@
         <v>2</v>
       </c>
       <c r="F22" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G22">
         <v>100</v>
       </c>
       <c r="H22" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="J22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10">
+        <v>-1</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -2219,19 +2391,31 @@
         <v>0</v>
       </c>
       <c r="F23" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G23">
         <v>200</v>
       </c>
       <c r="H23" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10">
+        <v>-1</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>7</v>
+      </c>
+      <c r="O23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -2248,19 +2432,22 @@
         <v>0</v>
       </c>
       <c r="F24" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G24">
         <v>200</v>
       </c>
       <c r="H24" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="J24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10">
+        <v>-1</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -2277,19 +2464,31 @@
         <v>0</v>
       </c>
       <c r="F25" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G25">
         <v>200</v>
       </c>
       <c r="H25" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10">
+        <v>-1</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>8</v>
+      </c>
+      <c r="O25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -2306,19 +2505,22 @@
         <v>-1</v>
       </c>
       <c r="F26" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G26">
         <v>400</v>
       </c>
       <c r="H26" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10">
+        <v>-1</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -2335,19 +2537,22 @@
         <v>-1</v>
       </c>
       <c r="F27" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G27">
         <v>200</v>
       </c>
       <c r="H27" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="J27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10">
+        <v>-1</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -2364,19 +2569,22 @@
         <v>-1</v>
       </c>
       <c r="F28" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G28">
         <v>200</v>
       </c>
       <c r="H28" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="J28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10">
+        <v>-1</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -2393,19 +2601,22 @@
         <v>-1</v>
       </c>
       <c r="F29" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G29">
         <v>200</v>
       </c>
       <c r="H29" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="J29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10">
+        <v>-1</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -2422,20 +2633,23 @@
         <v>2</v>
       </c>
       <c r="F30" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G30">
         <v>400</v>
       </c>
       <c r="H30" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="J30">
+        <v>-1</v>
+      </c>
+      <c r="K30">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="B2:O30">
+  <sortState ref="B2:P30">
     <sortCondition ref="C2:C30"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
import dottween & level up logic & bug fix
</commit_message>
<xml_diff>
--- a/Data/StoreItemDefine.xlsx
+++ b/Data/StoreItemDefine.xlsx
@@ -9,7 +9,20 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1443,7 +1456,7 @@
   <dimension ref="A1:W30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="T12" sqref="T12"/>
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -2415,7 +2428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:15">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -2445,6 +2458,15 @@
       </c>
       <c r="K24">
         <v>0</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>10</v>
+      </c>
+      <c r="O24">
+        <v>150</v>
       </c>
     </row>
     <row r="25" spans="1:15">

</xml_diff>

<commit_message>
forge page logic complete
</commit_message>
<xml_diff>
--- a/Data/StoreItemDefine.xlsx
+++ b/Data/StoreItemDefine.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="7440"/>
+    <workbookView windowHeight="16760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1548,8 +1548,8 @@
   <sheetPr/>
   <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="G30" workbookViewId="0">
-      <selection activeCell="I39" sqref="I39"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>

</xml_diff>